<commit_message>
Capstone Push June 17
</commit_message>
<xml_diff>
--- a/Excel Books/hot_streak.xlsx
+++ b/Excel Books/hot_streak.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\DM3PEPF00014031\EXCELCNV\093543d9-d49d-48d3-acf4-aa493596bf8d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D76C8DC5-1231-41E4-B2A0-6201775945F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C6B09DC-7466-43EA-AC69-D06D3DDA1797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" firstSheet="9" activeTab="9" xr2:uid="{0BA507BE-B26D-485F-88E6-6960AC2C82B3}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="56">
   <si>
     <t>Team</t>
   </si>
@@ -71,7 +71,7 @@
     <t>Rk</t>
   </si>
   <si>
-    <t>St Louis Blues</t>
+    <t>St. Louis Blues</t>
   </si>
   <si>
     <t>Chicago Blackhawks</t>
@@ -140,9 +140,6 @@
     <t>Edmonton Oilers</t>
   </si>
   <si>
-    <t>St. Louis Blues</t>
-  </si>
-  <si>
     <t>Columbus Blue Jackets</t>
   </si>
   <si>
@@ -194,6 +191,12 @@
     <t xml:space="preserve">Count of Teams </t>
   </si>
   <si>
+    <t>Worst Hot Streak coming into the playoffs to make the finals</t>
+  </si>
+  <si>
+    <t>St Louis Blues</t>
+  </si>
+  <si>
     <t>Finalist</t>
   </si>
   <si>
@@ -207,6 +210,9 @@
   </si>
   <si>
     <t>Missed</t>
+  </si>
+  <si>
+    <t>Highest Hot Streak to Not Make the Playoffs</t>
   </si>
 </sst>
 </file>
@@ -830,11 +836,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'All Seasons'!J1</c:f>
+              <c:f>'All Seasons'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -845,7 +851,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -878,31 +884,31 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Seasons'!J2:J6</c:f>
+              <c:f>'All Seasons'!$J$2:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.56941176470588228</c:v>
+                  <c:v>0.57111111111111101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61411764705882355</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58181818181818179</c:v>
+                  <c:v>0.58111111111111113</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56857142857142884</c:v>
+                  <c:v>0.57388888888888911</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42399999999999999</c:v>
+                  <c:v>0.41246376811594193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{F07F5134-C583-425E-9CF3-CC5E4002E671}"/>
+              <c16:uniqueId val="{0000000C-074B-4099-B159-6738CA544057}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -916,73 +922,74 @@
         </c:dLbls>
         <c:gapWidth val="33"/>
         <c:overlap val="-30"/>
-        <c:axId val="1578041352"/>
-        <c:axId val="1578043400"/>
+        <c:axId val="82705415"/>
+        <c:axId val="82644487"/>
       </c:barChart>
+      <c:valAx>
+        <c:axId val="82644487"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="82705415"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:catAx>
-        <c:axId val="1578041352"/>
+        <c:axId val="82705415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Round</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1018,124 +1025,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1578043400"/>
+        <c:crossAx val="82644487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
-      <c:valAx>
-        <c:axId val="1578043400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Win %</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1578041352"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1728,20 +1624,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2" descr="Chart type: Clustered Column. 'Score'&#10;&#10;Description automatically generated">
+        <xdr:cNvPr id="2" name="Chart 2" descr="Chart type: Clustered Column. 'Score'&#10;&#10;Description automatically generated">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D07B886D-5A8D-CCAE-0B91-7FF9FB285739}"/>
@@ -2064,12 +1960,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD9FD1F-09AC-47B3-A895-4D73BC9E68A5}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2123,13 +2020,13 @@
         <f>C2/(C2+D2+E2)</f>
         <v>0.76</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2">
         <f>_xlfn.XLOOKUP(B2,$J$2:$J$17,$I$2:$I$17,"Miss")</f>
-        <v>Miss</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <f>IF(G2&lt;=2,5,IF(G2&lt;=4,3,IF(G2&lt;=8,2,IF(G2&lt;=16,1,0))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2590,7 +2487,7 @@
         <v>14</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2598,7 +2495,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>13</v>
@@ -2625,7 +2522,7 @@
         <v>15</v>
       </c>
       <c r="J16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2633,7 +2530,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>13</v>
@@ -2726,7 +2623,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>12</v>
@@ -2842,7 +2739,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>11</v>
@@ -2871,7 +2768,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>11</v>
@@ -2929,7 +2826,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27">
         <v>11</v>
@@ -3016,7 +2913,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -3074,7 +2971,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -3103,7 +3000,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -3134,10 +3031,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B5C172-EE33-4F89-9111-78D1FAFAD393}">
-  <dimension ref="A1:K283"/>
+  <dimension ref="A1:P283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J6"/>
+      <selection activeCell="N13" sqref="N13:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3145,63 +3042,67 @@
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>2015</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1">
         <v>0.76</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" s="3">
         <f>AVERAGEIF($D$2:$D$283,I2,$C$2:$C$283)</f>
-        <v>0.56941176470588228</v>
+        <v>0.57111111111111101</v>
       </c>
       <c r="K2">
         <f>COUNTIF($D$2:$D$283,I2)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -3215,21 +3116,33 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I3">
         <v>3</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ref="J3:J6" si="0">AVERAGEIF($D$2:$D$283,I3,$C$2:$C$283)</f>
-        <v>0.61411764705882355</v>
+        <v>0.62</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K6" si="1">COUNTIF($D$2:$D$283,I3)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>18</v>
+      </c>
+      <c r="N3">
+        <f>INDEX(A2:A281,MATCH(_xlfn.MINIFS($C$2:$C$281,$D$2:$D$281,$I$2),$C$2:$C$281,0))</f>
+        <v>2015</v>
+      </c>
+      <c r="O3" t="str">
+        <f>INDEX(B2:B281,MATCH(_xlfn.MINIFS($C$2:$C$281,$D$2:$D$281,$I$2),$C$2:$C$281,0))</f>
+        <v>Chicago Blackhawks</v>
+      </c>
+      <c r="P3">
+        <f>_xlfn.MINIFS(C2:C283,D2:D283,I2)</f>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -3243,21 +3156,21 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" si="0"/>
-        <v>0.58181818181818179</v>
+        <v>0.58111111111111113</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>2015</v>
       </c>
@@ -3271,21 +3184,21 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="0"/>
-        <v>0.56857142857142884</v>
+        <v>0.57388888888888911</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>2015</v>
       </c>
@@ -3299,21 +3212,24 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>0.42399999999999999</v>
+        <v>0.41246376811594193</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>138</v>
+      </c>
+      <c r="N6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3327,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -3340,8 +3256,20 @@
       <c r="D8" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="N8">
+        <f>INDEX(A2:A281,MATCH(_xlfn.MAXIFS($C$2:$C$281,$D$2:$D$281,$I$6),$C$2:$C$281,0))</f>
+        <v>2016</v>
+      </c>
+      <c r="O8" t="str">
+        <f>INDEX(B2:B281,MATCH(_xlfn.MAXIFS($C$2:$C$281,$D$2:$D$281,$I$6),$C$2:$C$281,0))</f>
+        <v>St. Louis Blues</v>
+      </c>
+      <c r="P8">
+        <f>_xlfn.MAXIFS(C2:C283,D2:D283,I6)</f>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -3355,7 +3283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>2015</v>
       </c>
@@ -3369,7 +3297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -3383,7 +3311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -3397,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -3411,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>2015</v>
       </c>
@@ -3425,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -3439,12 +3367,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>2015</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1">
         <v>0.52</v>
@@ -3458,7 +3386,7 @@
         <v>2015</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1">
         <v>0.52</v>
@@ -3500,7 +3428,7 @@
         <v>2015</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1">
         <v>0.48</v>
@@ -3556,7 +3484,7 @@
         <v>2015</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1">
         <v>0.44</v>
@@ -3570,7 +3498,7 @@
         <v>2015</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1">
         <v>0.44</v>
@@ -3598,7 +3526,7 @@
         <v>2015</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="1">
         <v>0.44</v>
@@ -3640,7 +3568,7 @@
         <v>2015</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1">
         <v>0.36</v>
@@ -3668,7 +3596,7 @@
         <v>2015</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="1">
         <v>0.24</v>
@@ -3682,7 +3610,7 @@
         <v>2015</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1">
         <v>0.2</v>
@@ -3696,7 +3624,7 @@
         <v>2016</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="1">
         <v>0.76</v>
@@ -3716,7 +3644,7 @@
         <v>0.72</v>
       </c>
       <c r="D35" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3738,7 +3666,7 @@
         <v>2016</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1">
         <v>0.64</v>
@@ -3780,7 +3708,7 @@
         <v>2016</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="1">
         <v>0.56000000000000005</v>
@@ -3822,7 +3750,7 @@
         <v>2016</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" s="1">
         <v>0.6</v>
@@ -3878,7 +3806,7 @@
         <v>2016</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" s="1">
         <v>0.48</v>
@@ -3948,7 +3876,7 @@
         <v>2016</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C52" s="1">
         <v>0.44</v>
@@ -3976,7 +3904,7 @@
         <v>2016</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C54" s="1">
         <v>0.44</v>
@@ -4060,7 +3988,7 @@
         <v>2016</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C60" s="1">
         <v>0.36</v>
@@ -4102,7 +4030,7 @@
         <v>2016</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C63" s="1">
         <v>0.32</v>
@@ -4186,13 +4114,13 @@
         <v>2017</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C69" s="1">
         <v>0.64</v>
       </c>
       <c r="D69" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -4200,7 +4128,7 @@
         <v>2017</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C70" s="1">
         <v>0.64</v>
@@ -4298,7 +4226,7 @@
         <v>2017</v>
       </c>
       <c r="B77" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C77" s="1">
         <v>0.56000000000000005</v>
@@ -4340,7 +4268,7 @@
         <v>2017</v>
       </c>
       <c r="B80" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C80" s="1">
         <v>0.52</v>
@@ -4368,7 +4296,7 @@
         <v>2017</v>
       </c>
       <c r="B82" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C82" s="1">
         <v>0.48</v>
@@ -4396,7 +4324,7 @@
         <v>2017</v>
       </c>
       <c r="B84" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C84" s="1">
         <v>0.48</v>
@@ -4452,7 +4380,7 @@
         <v>2017</v>
       </c>
       <c r="B88" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C88" s="1">
         <v>0.4</v>
@@ -4466,7 +4394,7 @@
         <v>2017</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C89" s="1">
         <v>0.36</v>
@@ -4480,7 +4408,7 @@
         <v>2017</v>
       </c>
       <c r="B90" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C90" s="1">
         <v>0.32</v>
@@ -4522,7 +4450,7 @@
         <v>2017</v>
       </c>
       <c r="B93" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C93" s="1">
         <v>0.16</v>
@@ -4564,7 +4492,7 @@
         <v>2018</v>
       </c>
       <c r="B96" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C96" s="1">
         <v>0.72</v>
@@ -4592,7 +4520,7 @@
         <v>2018</v>
       </c>
       <c r="B98" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C98" s="1">
         <v>0.64</v>
@@ -4606,7 +4534,7 @@
         <v>2018</v>
       </c>
       <c r="B99" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C99" s="1">
         <v>0.64</v>
@@ -4676,7 +4604,7 @@
         <v>2018</v>
       </c>
       <c r="B104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C104" s="1">
         <v>0.56000000000000005</v>
@@ -4690,7 +4618,7 @@
         <v>2018</v>
       </c>
       <c r="B105" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C105" s="1">
         <v>0.56000000000000005</v>
@@ -4704,7 +4632,7 @@
         <v>2018</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C106" s="1">
         <v>0.6</v>
@@ -4732,7 +4660,7 @@
         <v>2018</v>
       </c>
       <c r="B108" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C108" s="1">
         <v>0.6</v>
@@ -4746,7 +4674,7 @@
         <v>2018</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C109" s="1">
         <v>0.56000000000000005</v>
@@ -4802,7 +4730,7 @@
         <v>2018</v>
       </c>
       <c r="B113" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C113" s="1">
         <v>0.4</v>
@@ -4900,7 +4828,7 @@
         <v>2018</v>
       </c>
       <c r="B120" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C120" s="1">
         <v>0.32</v>
@@ -4984,7 +4912,7 @@
         <v>2019</v>
       </c>
       <c r="B126" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C126" s="1">
         <v>0.68</v>
@@ -5026,13 +4954,13 @@
         <v>2019</v>
       </c>
       <c r="B129" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C129" s="1">
         <v>0.6</v>
       </c>
       <c r="D129" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -5054,7 +4982,7 @@
         <v>2019</v>
       </c>
       <c r="B131" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C131" s="1">
         <v>0.56000000000000005</v>
@@ -5082,7 +5010,7 @@
         <v>2019</v>
       </c>
       <c r="B133" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C133" s="1">
         <v>0.56000000000000005</v>
@@ -5124,7 +5052,7 @@
         <v>2019</v>
       </c>
       <c r="B136" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C136" s="1">
         <v>0.56000000000000005</v>
@@ -5166,7 +5094,7 @@
         <v>2019</v>
       </c>
       <c r="B139" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C139" s="1">
         <v>0.44</v>
@@ -5236,7 +5164,7 @@
         <v>2019</v>
       </c>
       <c r="B144" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C144" s="1">
         <v>0.48</v>
@@ -5320,7 +5248,7 @@
         <v>2019</v>
       </c>
       <c r="B150" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C150" s="1">
         <v>0.44</v>
@@ -5334,7 +5262,7 @@
         <v>2019</v>
       </c>
       <c r="B151" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C151" s="1">
         <v>0.4</v>
@@ -5390,7 +5318,7 @@
         <v>2019</v>
       </c>
       <c r="B155" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C155" s="1">
         <v>0.2</v>
@@ -5432,7 +5360,7 @@
         <v>2022</v>
       </c>
       <c r="B158" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C158" s="1">
         <v>0.76</v>
@@ -5460,13 +5388,13 @@
         <v>2022</v>
       </c>
       <c r="B160" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C160" s="1">
         <v>0.64</v>
       </c>
       <c r="D160" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -5474,7 +5402,7 @@
         <v>2022</v>
       </c>
       <c r="B161" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C161" s="1">
         <v>0.68</v>
@@ -5530,7 +5458,7 @@
         <v>2022</v>
       </c>
       <c r="B165" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C165" s="1">
         <v>0.56000000000000005</v>
@@ -5684,7 +5612,7 @@
         <v>2022</v>
       </c>
       <c r="B176" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C176" s="1">
         <v>0.48</v>
@@ -5712,7 +5640,7 @@
         <v>2022</v>
       </c>
       <c r="B178" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C178" s="1">
         <v>0.36</v>
@@ -5726,7 +5654,7 @@
         <v>2022</v>
       </c>
       <c r="B179" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C179" s="1">
         <v>0.4</v>
@@ -5768,7 +5696,7 @@
         <v>2022</v>
       </c>
       <c r="B182" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C182" s="1">
         <v>0.28000000000000003</v>
@@ -5796,7 +5724,7 @@
         <v>2022</v>
       </c>
       <c r="B184" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C184" s="1">
         <v>0.28000000000000003</v>
@@ -5810,7 +5738,7 @@
         <v>2022</v>
       </c>
       <c r="B185" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C185" s="1">
         <v>0.24</v>
@@ -5838,7 +5766,7 @@
         <v>2022</v>
       </c>
       <c r="B187" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C187" s="1">
         <v>0.28000000000000003</v>
@@ -5852,7 +5780,7 @@
         <v>2023</v>
       </c>
       <c r="B188" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C188" s="1">
         <v>0.84</v>
@@ -5978,7 +5906,7 @@
         <v>2023</v>
       </c>
       <c r="B197" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C197" s="1">
         <v>0.6</v>
@@ -5992,7 +5920,7 @@
         <v>2023</v>
       </c>
       <c r="B198" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C198" s="1">
         <v>0.6</v>
@@ -6048,7 +5976,7 @@
         <v>2023</v>
       </c>
       <c r="B202" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C202" s="1">
         <v>0.56000000000000005</v>
@@ -6090,7 +6018,7 @@
         <v>2023</v>
       </c>
       <c r="B205" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C205" s="1">
         <v>0.52</v>
@@ -6104,7 +6032,7 @@
         <v>2023</v>
       </c>
       <c r="B206" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C206" s="1">
         <v>0.48</v>
@@ -6132,13 +6060,13 @@
         <v>2023</v>
       </c>
       <c r="B208" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C208" s="1">
         <v>0.44</v>
       </c>
       <c r="D208" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -6174,7 +6102,7 @@
         <v>2023</v>
       </c>
       <c r="B211" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C211" s="1">
         <v>0.32</v>
@@ -6188,7 +6116,7 @@
         <v>2023</v>
       </c>
       <c r="B212" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C212" s="1">
         <v>0.36</v>
@@ -6202,7 +6130,7 @@
         <v>2023</v>
       </c>
       <c r="B213" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C213" s="1">
         <v>0.28000000000000003</v>
@@ -6272,7 +6200,7 @@
         <v>2023</v>
       </c>
       <c r="B218" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C218" s="1">
         <v>0.2</v>
@@ -6412,7 +6340,7 @@
         <v>2024</v>
       </c>
       <c r="B228" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C228" s="1">
         <v>0.6</v>
@@ -6454,7 +6382,7 @@
         <v>2024</v>
       </c>
       <c r="B231" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C231" s="1">
         <v>0.52</v>
@@ -6468,7 +6396,7 @@
         <v>2024</v>
       </c>
       <c r="B232" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C232" s="1">
         <v>0.52</v>
@@ -6496,7 +6424,7 @@
         <v>2024</v>
       </c>
       <c r="B234" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C234" s="1">
         <v>0.52</v>
@@ -6566,7 +6494,7 @@
         <v>2024</v>
       </c>
       <c r="B239" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C239" s="1">
         <v>0.52</v>
@@ -6580,7 +6508,7 @@
         <v>2024</v>
       </c>
       <c r="B240" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C240" s="1">
         <v>0.44</v>
@@ -6650,7 +6578,7 @@
         <v>2024</v>
       </c>
       <c r="B245" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C245" s="1">
         <v>0.4</v>
@@ -6664,7 +6592,7 @@
         <v>2024</v>
       </c>
       <c r="B246" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C246" s="1">
         <v>0.32</v>
@@ -6692,7 +6620,7 @@
         <v>2024</v>
       </c>
       <c r="B248" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C248" s="1">
         <v>0.36</v>
@@ -6706,7 +6634,7 @@
         <v>2024</v>
       </c>
       <c r="B249" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C249" s="1">
         <v>0.32</v>
@@ -6734,7 +6662,7 @@
         <v>2024</v>
       </c>
       <c r="B251" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C251" s="1">
         <v>0.16</v>
@@ -6748,13 +6676,13 @@
         <v>2025</v>
       </c>
       <c r="B252" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C252" s="1">
         <v>0.76</v>
       </c>
       <c r="D252" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -6944,7 +6872,7 @@
         <v>2025</v>
       </c>
       <c r="B266" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C266" s="1">
         <v>0.52</v>
@@ -6958,7 +6886,7 @@
         <v>2025</v>
       </c>
       <c r="B267" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C267" s="1">
         <v>0.52</v>
@@ -7000,7 +6928,7 @@
         <v>2025</v>
       </c>
       <c r="B270" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C270" s="1">
         <v>0.48</v>
@@ -7056,7 +6984,7 @@
         <v>2025</v>
       </c>
       <c r="B274" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C274" s="1">
         <v>0.44</v>
@@ -7070,7 +6998,7 @@
         <v>2025</v>
       </c>
       <c r="B275" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C275" s="1">
         <v>0.44</v>
@@ -7098,7 +7026,7 @@
         <v>2025</v>
       </c>
       <c r="B277" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C277" s="1">
         <v>0.44</v>
@@ -7140,7 +7068,7 @@
         <v>2025</v>
       </c>
       <c r="B280" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C280" s="1">
         <v>0.36</v>
@@ -7168,7 +7096,7 @@
         <v>2025</v>
       </c>
       <c r="B282" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C282" s="1">
         <v>0.24</v>
@@ -7182,7 +7110,7 @@
         <v>2025</v>
       </c>
       <c r="B283" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C283" s="1">
         <v>0.2</v>
@@ -7201,7 +7129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326F4991-2881-422E-9948-2659A6AB26CB}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H31"/>
     </sheetView>
   </sheetViews>
@@ -7244,7 +7172,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>19</v>
@@ -7271,7 +7199,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -7294,19 +7222,19 @@
         <f t="shared" ref="F3:F31" si="0">C3/(C3+D3+E3)</f>
         <v>0.72</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G3">
         <f t="shared" ref="G3:G31" si="1">_xlfn.XLOOKUP(B3,$L$2:$L$17,$K$2:$K$17,"Miss")</f>
-        <v>Miss</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H31" si="2">IF(G3&lt;=2,5,IF(G3&lt;=4,3,IF(G3&lt;=8,2,IF(G3&lt;=16,1,0))))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -7349,7 +7277,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -7376,7 +7304,7 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -7454,7 +7382,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>14</v>
@@ -7559,7 +7487,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11">
         <v>15</v>
@@ -7656,7 +7584,7 @@
         <v>12</v>
       </c>
       <c r="L13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -7691,7 +7619,7 @@
         <v>13</v>
       </c>
       <c r="L14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -7699,7 +7627,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>12</v>
@@ -7862,7 +7790,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20">
         <v>11</v>
@@ -7920,7 +7848,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22">
         <v>11</v>
@@ -8094,7 +8022,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>9</v>
@@ -8181,7 +8109,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31">
         <v>8</v>
@@ -8214,12 +8142,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34423AF-1DC0-4B20-A022-80F7904DCCB4}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8284,7 +8213,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -8447,13 +8376,13 @@
         <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
-      <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>Miss</v>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <v>6</v>
@@ -8467,7 +8396,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -8494,7 +8423,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -8564,7 +8493,7 @@
         <v>9</v>
       </c>
       <c r="L10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -8634,7 +8563,7 @@
         <v>11</v>
       </c>
       <c r="L12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -8712,7 +8641,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -8739,7 +8668,7 @@
         <v>14</v>
       </c>
       <c r="L15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -8817,7 +8746,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <v>13</v>
@@ -8875,7 +8804,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <v>12</v>
@@ -8933,7 +8862,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22">
         <v>12</v>
@@ -9049,7 +8978,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -9078,7 +9007,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>9</v>
@@ -9107,7 +9036,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -9194,7 +9123,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -9227,7 +9156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487DAD37-67C8-4E75-B3C0-92B27CFA3BF3}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H32"/>
     </sheetView>
   </sheetViews>
@@ -9340,7 +9269,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -9410,7 +9339,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -9445,7 +9374,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -9472,7 +9401,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -9507,7 +9436,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -9542,7 +9471,7 @@
         <v>8</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -9612,7 +9541,7 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -9620,7 +9549,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -9655,7 +9584,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>14</v>
@@ -9682,7 +9611,7 @@
         <v>12</v>
       </c>
       <c r="L13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -9690,7 +9619,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -9752,7 +9681,7 @@
         <v>14</v>
       </c>
       <c r="L15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -9760,7 +9689,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -9795,7 +9724,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>14</v>
@@ -10120,7 +10049,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -10269,7 +10198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFE0005-D3FE-42BC-9CEE-59E78BDA4199}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H32"/>
     </sheetView>
   </sheetViews>
@@ -10339,7 +10268,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -10347,7 +10276,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>17</v>
@@ -10374,7 +10303,7 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -10409,7 +10338,7 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -10467,13 +10396,13 @@
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>Miss</v>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>5</v>
@@ -10522,7 +10451,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>14</v>
@@ -10549,7 +10478,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -10592,7 +10521,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>14</v>
@@ -10697,7 +10626,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>14</v>
@@ -10802,7 +10731,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>11</v>
@@ -10829,7 +10758,7 @@
         <v>15</v>
       </c>
       <c r="L16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -10959,7 +10888,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21">
         <v>12</v>
@@ -11133,7 +11062,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27">
         <v>11</v>
@@ -11162,7 +11091,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -11278,7 +11207,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -11311,7 +11240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DCE6B1-6AA1-4C34-A0CC-93EACFC8C44A}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H33"/>
     </sheetView>
   </sheetViews>
@@ -11424,7 +11353,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>19</v>
@@ -11509,13 +11438,13 @@
         <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
-      <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>Miss</v>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6">
         <v>5</v>
@@ -11529,7 +11458,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7">
         <v>17</v>
@@ -11556,7 +11485,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -11626,7 +11555,7 @@
         <v>8</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -11661,7 +11590,7 @@
         <v>9</v>
       </c>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -11669,7 +11598,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>14</v>
@@ -11801,7 +11730,7 @@
         <v>13</v>
       </c>
       <c r="L14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -12030,7 +11959,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>12</v>
@@ -12088,7 +12017,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>9</v>
@@ -12117,7 +12046,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -12204,7 +12133,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -12262,7 +12191,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -12291,7 +12220,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>6</v>
@@ -12349,7 +12278,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>7</v>
@@ -12382,7 +12311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7EF753-89DE-4DD0-998D-60650108959E}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H33"/>
     </sheetView>
   </sheetViews>
@@ -12411,7 +12340,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -12425,7 +12354,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>21</v>
@@ -12627,7 +12556,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -12697,7 +12626,7 @@
         <v>8</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -12732,7 +12661,7 @@
         <v>9</v>
       </c>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -12740,7 +12669,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>15</v>
@@ -12775,7 +12704,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>15</v>
@@ -12872,7 +12801,7 @@
         <v>13</v>
       </c>
       <c r="L14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -12915,7 +12844,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>14</v>
@@ -13014,7 +12943,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>13</v>
@@ -13043,7 +12972,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>12</v>
@@ -13116,13 +13045,13 @@
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
-      <c r="G22" t="str">
-        <f t="shared" si="1"/>
-        <v>Miss</v>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -13188,7 +13117,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25">
         <v>8</v>
@@ -13217,7 +13146,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26">
         <v>9</v>
@@ -13246,7 +13175,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27">
         <v>7</v>
@@ -13391,7 +13320,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -13453,7 +13382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BF7D02-B50E-43C1-BB14-4D5E47066DFE}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H33"/>
     </sheetView>
   </sheetViews>
@@ -13523,7 +13452,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -13768,7 +13697,7 @@
         <v>8</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -13776,7 +13705,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>15</v>
@@ -13881,7 +13810,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13">
         <v>13</v>
@@ -13986,7 +13915,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>13</v>
@@ -14143,7 +14072,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21">
         <v>13</v>
@@ -14172,7 +14101,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>11</v>
@@ -14317,7 +14246,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -14346,7 +14275,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -14404,7 +14333,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -14433,7 +14362,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>8</v>
@@ -14491,7 +14420,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -14524,8 +14453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D186B5CA-65DB-482E-A48F-B3CC07D23F92}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14579,13 +14508,13 @@
         <f>C2/(C2+D2+E2)</f>
         <v>0.76</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2">
         <f>_xlfn.XLOOKUP(B2,$L$2:$L$17,$K$2:$K$17,"Miss")</f>
-        <v>Miss</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <f>IF(G2&lt;=2,5,IF(G2&lt;=4,3,IF(G2&lt;=8,2,IF(G2&lt;=16,1,0))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -14626,7 +14555,7 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -14906,7 +14835,7 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -15046,7 +14975,7 @@
         <v>14</v>
       </c>
       <c r="L15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -15054,7 +14983,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>13</v>
@@ -15089,7 +15018,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>13</v>
@@ -15182,7 +15111,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>12</v>
@@ -15298,7 +15227,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>11</v>
@@ -15327,7 +15256,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>11</v>
@@ -15385,7 +15314,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27">
         <v>11</v>
@@ -15472,7 +15401,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -15530,7 +15459,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -15559,7 +15488,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33">
         <v>5</v>

</xml_diff>